<commit_message>
Added boost::unordered_set & spp::sparse_hash_set (boost::flat_hash added to test, but too slow and not included into results)
</commit_message>
<xml_diff>
--- a/SetsCompare.xlsx
+++ b/SetsCompare.xlsx
@@ -12,10 +12,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Best_Hit">Sheet1!$D$14</definedName>
-    <definedName name="Best_Miss">Sheet1!$E$14</definedName>
-    <definedName name="Best_Population">Sheet1!$B$14</definedName>
-    <definedName name="Best_Population_Hit">Sheet1!$C$14</definedName>
+    <definedName name="Best_Hit">Sheet1!$D$18</definedName>
+    <definedName name="Best_Miss">Sheet1!$E$18</definedName>
+    <definedName name="Best_Population">Sheet1!$B$18</definedName>
+    <definedName name="Best_Population_Hit">Sheet1!$C$18</definedName>
     <definedName name="Best_Size">Sheet1!$E$1</definedName>
     <definedName name="DataSize">Sheet1!$F$2</definedName>
     <definedName name="PopulateTime">Sheet1!$B$2</definedName>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Search</t>
   </si>
@@ -122,12 +122,27 @@
   </si>
   <si>
     <t>Used, ratio</t>
+  </si>
+  <si>
+    <t>boost::unordered_set</t>
+  </si>
+  <si>
+    <t>spp::sparse_hash_set</t>
+  </si>
+  <si>
+    <t>boost::unordered_set pool</t>
+  </si>
+  <si>
+    <t>spp::sparse_hash_set pool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -169,10 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,12 +496,12 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -505,468 +520,468 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>10.8</v>
-      </c>
-      <c r="C3" s="3">
-        <v>6.13</v>
-      </c>
-      <c r="D3" s="3">
-        <v>4.79</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4.5999999999999996</v>
+        <v>32</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10.109</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5.2030000000000003</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5.25</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.41</v>
       </c>
       <c r="F3" s="2">
-        <v>1158720</v>
+        <v>829120</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G13" si="0">I3-K3+M3</f>
-        <v>1486626824</v>
+        <f t="shared" ref="G3:G17" si="0">I3-K3+M3</f>
+        <v>857488598</v>
       </c>
       <c r="H3" s="2">
-        <v>20000020</v>
+        <v>20000022</v>
       </c>
       <c r="I3" s="2">
-        <v>1553734808</v>
+        <v>882654576</v>
       </c>
       <c r="J3" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K3" s="2">
-        <v>67107984</v>
+        <v>25165978</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="1">
-        <f>B3/Best_Population</f>
-        <v>2.8800000000000003</v>
+        <f t="shared" ref="N3:N17" si="1">B3/Best_Population</f>
+        <v>3.0230263157894739</v>
       </c>
       <c r="O3" s="1">
-        <f>C3/Best_Population_Hit</f>
-        <v>2.0298013245033113</v>
+        <f t="shared" ref="O3:O17" si="2">C3/Best_Population_Hit</f>
+        <v>1.9889143730886851</v>
       </c>
       <c r="P3" s="1">
-        <f>F3*1024/Best_Size</f>
-        <v>7.4158080000000002</v>
+        <f t="shared" ref="P3:P17" si="3">F3*1024/Best_Size</f>
+        <v>5.306368</v>
       </c>
       <c r="Q3" s="1">
-        <f>G3/Best_Size</f>
-        <v>9.2914176499999996</v>
+        <f t="shared" ref="Q3:Q17" si="4">G3/Best_Size</f>
+        <v>5.3593037375000003</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7.6909999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.3250000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>8.7100000000000009</v>
-      </c>
-      <c r="C4" s="3">
-        <v>8.02</v>
-      </c>
-      <c r="D4" s="3">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8.23</v>
-      </c>
       <c r="F4" s="2">
-        <v>222608</v>
+        <v>379532</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>209725832</v>
+        <v>1556512798</v>
       </c>
       <c r="H4" s="2">
-        <v>790121</v>
+        <v>19786299</v>
       </c>
       <c r="I4" s="2">
-        <v>209726160</v>
+        <v>1742233944</v>
       </c>
       <c r="J4" s="2">
-        <v>5</v>
+        <v>17689276</v>
       </c>
       <c r="K4" s="2">
-        <v>328</v>
+        <v>185721146</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="1">
-        <f>B4/Best_Population</f>
-        <v>2.3226666666666671</v>
+        <f t="shared" si="1"/>
+        <v>2.2999401913875599</v>
       </c>
       <c r="O4" s="1">
-        <f>C4/Best_Population_Hit</f>
-        <v>2.6556291390728477</v>
+        <f t="shared" si="2"/>
+        <v>1.6532874617737003</v>
       </c>
       <c r="P4" s="1">
-        <f>F4*1024/Best_Size</f>
-        <v>1.4246912</v>
+        <f t="shared" si="3"/>
+        <v>2.4290048</v>
       </c>
       <c r="Q4" s="1">
-        <f>G4/Best_Size</f>
-        <v>1.3107864499999999</v>
+        <f t="shared" si="4"/>
+        <v>9.7282049874999998</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>13.23</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4.26</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9.4939999999999998</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.2279999999999998</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.0869999999999997</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3.9089999999999998</v>
       </c>
       <c r="F5" s="2">
-        <v>253104</v>
+        <v>1156796</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>369575293</v>
+        <v>1486626824</v>
       </c>
       <c r="H5" s="2">
-        <v>21</v>
+        <v>20000020</v>
       </c>
       <c r="I5" s="2">
-        <v>22369776</v>
+        <v>1553734808</v>
       </c>
       <c r="J5" s="2">
-        <v>699080</v>
+        <v>18</v>
       </c>
       <c r="K5" s="2">
-        <v>27542571</v>
-      </c>
-      <c r="L5" s="2">
-        <v>46843511</v>
-      </c>
-      <c r="M5" s="2">
-        <v>374748088</v>
-      </c>
+        <v>67107984</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="1">
-        <f>B5/Best_Population</f>
-        <v>3.528</v>
+        <f t="shared" si="1"/>
+        <v>2.839114832535885</v>
       </c>
       <c r="O5" s="1">
-        <f>C5/Best_Population_Hit</f>
-        <v>1.7218543046357617</v>
+        <f t="shared" si="2"/>
+        <v>1.9984709480122322</v>
       </c>
       <c r="P5" s="1">
-        <f>F5*1024/Best_Size</f>
-        <v>1.6198656</v>
+        <f t="shared" si="3"/>
+        <v>7.4034943999999996</v>
       </c>
       <c r="Q5" s="1">
-        <f>G5/Best_Size</f>
-        <v>2.3098455812499998</v>
+        <f t="shared" si="4"/>
+        <v>9.2914176499999996</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3.75</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3.02</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2.94</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.09</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.7229999999999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.1440000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>7.2069999999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>7.2569999999999997</v>
       </c>
       <c r="F6" s="2">
-        <v>792460</v>
+        <v>220700</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>1006632736</v>
+        <v>209725832</v>
       </c>
       <c r="H6" s="2">
-        <v>22</v>
+        <v>790121</v>
       </c>
       <c r="I6" s="2">
-        <v>1073741568</v>
+        <v>209726160</v>
       </c>
       <c r="J6" s="2">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="K6" s="2">
-        <v>67108832</v>
+        <v>328</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="1">
-        <f>B6/Best_Population</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2.3095095693779903</v>
       </c>
       <c r="O6" s="1">
-        <f>C6/Best_Population_Hit</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>2.7308868501529053</v>
       </c>
       <c r="P6" s="1">
-        <f>F6*1024/Best_Size</f>
-        <v>5.0717439999999998</v>
+        <f t="shared" si="3"/>
+        <v>1.41248</v>
       </c>
       <c r="Q6" s="1">
-        <f>G6/Best_Size</f>
-        <v>6.2914545999999998</v>
+        <f t="shared" si="4"/>
+        <v>1.3107864499999999</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3.87</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3.28</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3.29</v>
-      </c>
-      <c r="E7" s="3">
-        <v>3.8</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>11.756</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.556</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4.5460000000000003</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3.722</v>
       </c>
       <c r="F7" s="2">
-        <v>792456</v>
+        <v>252420</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>1040187152</v>
+        <v>369575293</v>
       </c>
       <c r="H7" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2">
-        <v>1073741568</v>
+        <v>22369776</v>
       </c>
       <c r="J7" s="2">
-        <v>21</v>
+        <v>699080</v>
       </c>
       <c r="K7" s="2">
-        <v>33554416</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+        <v>27542571</v>
+      </c>
+      <c r="L7" s="2">
+        <v>46843511</v>
+      </c>
+      <c r="M7" s="2">
+        <v>374748088</v>
+      </c>
       <c r="N7" s="1">
-        <f>B7/Best_Population</f>
-        <v>1.032</v>
+        <f t="shared" si="1"/>
+        <v>3.5155502392344498</v>
       </c>
       <c r="O7" s="1">
-        <f>C7/Best_Population_Hit</f>
-        <v>1.0860927152317881</v>
+        <f t="shared" si="2"/>
+        <v>1.7415902140672783</v>
       </c>
       <c r="P7" s="1">
-        <f>F7*1024/Best_Size</f>
-        <v>5.0717184</v>
+        <f t="shared" si="3"/>
+        <v>1.615488</v>
       </c>
       <c r="Q7" s="1">
-        <f>G7/Best_Size</f>
-        <v>6.5011697000000002</v>
+        <f t="shared" si="4"/>
+        <v>2.3098455812499998</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3">
-        <v>7.07</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3.16</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3.69</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3.3439999999999999</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.5510000000000002</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.6970000000000001</v>
       </c>
       <c r="F8" s="2">
-        <v>792444</v>
+        <v>790280</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>1040187483</v>
+        <v>1006632736</v>
       </c>
       <c r="H8" s="2">
         <v>22</v>
       </c>
       <c r="I8" s="2">
-        <v>1073741920</v>
+        <v>1073741568</v>
       </c>
       <c r="J8" s="2">
         <v>21</v>
       </c>
       <c r="K8" s="2">
-        <v>33554437</v>
+        <v>67108832</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="1">
-        <f>B8/Best_Population</f>
-        <v>1.8853333333333333</v>
+        <f t="shared" ref="N8:N13" si="5">B8/Best_Population</f>
+        <v>1</v>
       </c>
       <c r="O8" s="1">
-        <f>C8/Best_Population_Hit</f>
-        <v>1.0397350993377483</v>
+        <f t="shared" ref="O8:O13" si="6">C8/Best_Population_Hit</f>
+        <v>1</v>
       </c>
       <c r="P8" s="1">
-        <f>F8*1024/Best_Size</f>
-        <v>5.0716416000000004</v>
+        <f t="shared" ref="P8:P13" si="7">F8*1024/Best_Size</f>
+        <v>5.0577920000000001</v>
       </c>
       <c r="Q8" s="1">
-        <f>G8/Best_Size</f>
-        <v>6.5011717687499999</v>
+        <f t="shared" ref="Q8:Q13" si="8">G8/Best_Size</f>
+        <v>6.2914545999999998</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3">
-        <v>7.04</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3.21</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3.22</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3.76</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.843</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.9060000000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3.3460000000000001</v>
       </c>
       <c r="F9" s="2">
-        <v>792456</v>
+        <v>790284</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>1040187483</v>
+        <v>1040187152</v>
       </c>
       <c r="H9" s="2">
         <v>22</v>
       </c>
       <c r="I9" s="2">
-        <v>1073741920</v>
+        <v>1073741568</v>
       </c>
       <c r="J9" s="2">
         <v>21</v>
       </c>
       <c r="K9" s="2">
-        <v>33554437</v>
+        <v>33554416</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="1">
-        <f>B9/Best_Population</f>
-        <v>1.8773333333333333</v>
+        <f t="shared" si="5"/>
+        <v>1.0062799043062203</v>
       </c>
       <c r="O9" s="1">
-        <f>C9/Best_Population_Hit</f>
-        <v>1.0629139072847682</v>
+        <f t="shared" si="6"/>
+        <v>1.0867737003058104</v>
       </c>
       <c r="P9" s="1">
-        <f>F9*1024/Best_Size</f>
-        <v>5.0717184</v>
+        <f t="shared" si="7"/>
+        <v>5.0578175999999999</v>
       </c>
       <c r="Q9" s="1">
-        <f>G9/Best_Size</f>
-        <v>6.5011717687499999</v>
+        <f t="shared" si="8"/>
+        <v>6.5011697000000002</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3">
-        <v>7.96</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3.38</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3.35</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4.04</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>6.1929999999999996</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.7709999999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.7519999999999998</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3.2330000000000001</v>
       </c>
       <c r="F10" s="2">
-        <v>1186184</v>
+        <v>790284</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>1577058443</v>
+        <v>1040187483</v>
       </c>
       <c r="H10" s="2">
         <v>22</v>
       </c>
       <c r="I10" s="2">
-        <v>1610612880</v>
+        <v>1073741920</v>
       </c>
       <c r="J10" s="2">
         <v>21</v>
@@ -977,204 +992,418 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="1">
-        <f>B10/Best_Population</f>
-        <v>2.1226666666666665</v>
+        <f t="shared" si="5"/>
+        <v>1.8519736842105263</v>
       </c>
       <c r="O10" s="1">
-        <f>C10/Best_Population_Hit</f>
-        <v>1.119205298013245</v>
+        <f t="shared" si="6"/>
+        <v>1.0592507645259939</v>
       </c>
       <c r="P10" s="1">
-        <f>F10*1024/Best_Size</f>
-        <v>7.5915775999999999</v>
+        <f t="shared" si="7"/>
+        <v>5.0578175999999999</v>
       </c>
       <c r="Q10" s="1">
-        <f>G10/Best_Size</f>
-        <v>9.8566152687499997</v>
+        <f t="shared" si="8"/>
+        <v>6.5011717687499999</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3">
-        <v>30.81</v>
-      </c>
-      <c r="C11" s="3">
-        <v>31.87</v>
-      </c>
-      <c r="D11" s="3">
-        <v>31.45</v>
-      </c>
-      <c r="E11" s="3">
-        <v>34.56</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6.1710000000000003</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.7549999999999999</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.7530000000000001</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3.2269999999999999</v>
       </c>
       <c r="F11" s="2">
-        <v>947928</v>
+        <v>790280</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>800000040</v>
+        <v>1040187483</v>
       </c>
       <c r="H11" s="2">
-        <v>20000001</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2">
-        <v>800000040</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+        <v>1073741920</v>
+      </c>
+      <c r="J11" s="2">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2">
+        <v>33554437</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="1">
-        <f>B11/Best_Population</f>
-        <v>8.2159999999999993</v>
+        <f t="shared" si="5"/>
+        <v>1.8453947368421053</v>
       </c>
       <c r="O11" s="1">
-        <f>C11/Best_Population_Hit</f>
-        <v>10.552980132450331</v>
+        <f t="shared" si="6"/>
+        <v>1.0531345565749235</v>
       </c>
       <c r="P11" s="1">
-        <f>F11*1024/Best_Size</f>
-        <v>6.0667391999999998</v>
+        <f t="shared" si="7"/>
+        <v>5.0577920000000001</v>
       </c>
       <c r="Q11" s="1">
-        <f>G11/Best_Size</f>
-        <v>5.0000002500000003</v>
+        <f t="shared" si="8"/>
+        <v>6.5011717687499999</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3">
-        <v>9.68</v>
-      </c>
-      <c r="C12" s="3">
-        <v>6.13</v>
-      </c>
-      <c r="D12" s="3">
-        <v>4.79</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4.5999999999999996</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6.7480000000000002</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.8660000000000001</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.8849999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.4670000000000001</v>
       </c>
       <c r="F12" s="2">
-        <v>1533260</v>
+        <v>1183880</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>1553858240</v>
+        <v>1577058443</v>
       </c>
       <c r="H12" s="2">
-        <v>29472</v>
+        <v>22</v>
       </c>
       <c r="I12" s="2">
-        <v>1553858240</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+        <v>1610612880</v>
+      </c>
+      <c r="J12" s="2">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2">
+        <v>33554437</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="1">
-        <f>B12/Best_Population</f>
-        <v>2.5813333333333333</v>
+        <f t="shared" si="5"/>
+        <v>2.0179425837320575</v>
       </c>
       <c r="O12" s="1">
-        <f>C12/Best_Population_Hit</f>
-        <v>2.0298013245033113</v>
+        <f t="shared" si="6"/>
+        <v>1.095565749235474</v>
       </c>
       <c r="P12" s="1">
-        <f>F12*1024/Best_Size</f>
-        <v>9.8128639999999994</v>
+        <f t="shared" si="7"/>
+        <v>7.5768319999999996</v>
       </c>
       <c r="Q12" s="1">
-        <f>G12/Best_Size</f>
-        <v>9.7116140000000009</v>
+        <f t="shared" si="8"/>
+        <v>9.8566152687499997</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3">
-        <v>28.62</v>
-      </c>
-      <c r="C13" s="3">
-        <v>31.87</v>
-      </c>
-      <c r="D13" s="3">
-        <v>31.45</v>
-      </c>
-      <c r="E13" s="3">
-        <v>34.56</v>
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>26.606999999999999</v>
+      </c>
+      <c r="C13" s="4">
+        <v>27.100999999999999</v>
+      </c>
+      <c r="D13" s="4">
+        <v>27.015999999999998</v>
+      </c>
+      <c r="E13" s="4">
+        <v>29.15</v>
       </c>
       <c r="F13" s="2">
-        <v>805288</v>
+        <v>946020</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>800998300</v>
+        <v>800000040</v>
       </c>
       <c r="H13" s="2">
-        <v>49141</v>
+        <v>20000001</v>
       </c>
       <c r="I13" s="2">
-        <v>800998300</v>
+        <v>800000040</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="1">
-        <f>B13/Best_Population</f>
-        <v>7.6320000000000006</v>
+        <f t="shared" si="5"/>
+        <v>7.9566387559808618</v>
       </c>
       <c r="O13" s="1">
-        <f>C13/Best_Population_Hit</f>
-        <v>10.552980132450331</v>
+        <f t="shared" si="6"/>
+        <v>10.359709480122323</v>
       </c>
       <c r="P13" s="1">
-        <f>F13*1024/Best_Size</f>
-        <v>5.1538431999999998</v>
+        <f t="shared" si="7"/>
+        <v>6.0545280000000004</v>
       </c>
       <c r="Q13" s="1">
-        <f>G13/Best_Size</f>
-        <v>5.0062393749999998</v>
+        <f t="shared" si="8"/>
+        <v>5.0000002500000003</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9.1389999999999993</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4.9119999999999999</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4.8650000000000002</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5.8689999999999998</v>
+      </c>
+      <c r="F14" s="2">
+        <v>875988</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>882778892</v>
+      </c>
+      <c r="H14" s="2">
+        <v>29471</v>
+      </c>
+      <c r="I14" s="2">
+        <v>882778892</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7329545454545454</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8776758409785932</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>5.6063232000000003</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="4"/>
+        <v>5.5173680750000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="4">
+        <v>6.2050000000000001</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4.5659999999999998</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4.3789999999999996</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3.0619999999999998</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1747052</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>1747721408</v>
+      </c>
+      <c r="H15" s="2">
+        <v>101060</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1747721408</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8555622009569379</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7454128440366972</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="3"/>
+        <v>11.1811328</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="4"/>
+        <v>10.923258799999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4.7629999999999999</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.8010000000000002</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.738</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1531348</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>1553858240</v>
+      </c>
+      <c r="H16" s="2">
+        <v>29472</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1553858240</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="1">
+        <f t="shared" si="1"/>
+        <v>2.526913875598086</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8207186544342506</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="3"/>
+        <v>9.8006271999999992</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="4"/>
+        <v>9.7116140000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4">
+        <v>24.640999999999998</v>
+      </c>
+      <c r="C17" s="4">
+        <v>25.765999999999998</v>
+      </c>
+      <c r="D17" s="4">
+        <v>25.029</v>
+      </c>
+      <c r="E17" s="4">
+        <v>27.431999999999999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>803352</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>800998300</v>
+      </c>
+      <c r="H17" s="2">
+        <v>49141</v>
+      </c>
+      <c r="I17" s="2">
+        <v>800998300</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="1">
+        <f t="shared" si="1"/>
+        <v>7.3687200956937797</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="2"/>
+        <v>9.8493883792048926</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="3"/>
+        <v>5.1414527999999997</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="4"/>
+        <v>5.0062393749999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3">
-        <f>MIN(B3:B13)</f>
-        <v>3.75</v>
-      </c>
-      <c r="C14" s="3">
-        <f>MIN(C3:C13)</f>
-        <v>3.02</v>
-      </c>
-      <c r="D14" s="3">
-        <f>MIN(D3:D13)</f>
-        <v>2.94</v>
-      </c>
-      <c r="E14" s="3">
-        <f>MIN(E3:E13)</f>
-        <v>3.09</v>
-      </c>
-      <c r="F14" s="2">
-        <f>MIN(F3:F13)</f>
-        <v>222608</v>
-      </c>
-      <c r="G14" s="2">
-        <f>MIN(G3:G13)</f>
+      <c r="B18" s="4">
+        <f>MIN(B3:B17)</f>
+        <v>3.3439999999999999</v>
+      </c>
+      <c r="C18" s="4">
+        <f>MIN(C3:C17)</f>
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="D18" s="4">
+        <f>MIN(D3:D17)</f>
+        <v>2.5510000000000002</v>
+      </c>
+      <c r="E18" s="4">
+        <f>MIN(E3:E17)</f>
+        <v>2.6970000000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <f>MIN(F3:F17)</f>
+        <v>220700</v>
+      </c>
+      <c r="G18" s="2">
+        <f>MIN(G3:G17)</f>
         <v>209725832</v>
       </c>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="2">
-        <f>I19-K19+M19</f>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="G23" s="2">
+        <f>I23-K23+M23</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>